<commit_message>
Actualización automática: 2025-06-22 11:03:27.535522
</commit_message>
<xml_diff>
--- a/CONTROL REEMBOLSOS.xlsx
+++ b/CONTROL REEMBOLSOS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Respaldo usuario\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seidor.ANALYTICS-EC001\Downloads\TRABAJOS_EXTRAS\TESIS_RUTH_AXEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F238845-E707-4DCA-8396-1B59E4187CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE43FAE0-59FF-4310-8D5C-7EAF5620D551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REEMBOLSOS 2024" sheetId="1" r:id="rId1"/>
@@ -26,12 +26,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6142" uniqueCount="1476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6149" uniqueCount="1479">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -4459,6 +4470,15 @@
   </si>
   <si>
     <t>CARMEN SOTO</t>
+  </si>
+  <si>
+    <t>FREDDY QUIMIS</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>esto es un test de actualizacion</t>
   </si>
 </sst>
 </file>
@@ -4466,8 +4486,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;\-#,##0.00"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;$&quot;* #,##0.00_ ;_ &quot;$&quot;* \-#,##0.00_ ;_ &quot;$&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;\-#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_ &quot;$&quot;* #,##0.00_ ;_ &quot;$&quot;* \-#,##0.00_ ;_ &quot;$&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -4692,7 +4712,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -4759,13 +4779,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4789,13 +4809,13 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="12" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="12" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4815,7 +4835,14 @@
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="120">
+  <dxfs count="108">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -4829,7 +4856,46 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4848,6 +4914,20 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color auto="1"/>
       </font>
@@ -4858,6 +4938,38 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
@@ -4874,6 +4986,23 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
@@ -4883,6 +5012,68 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4937,6 +5128,69 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -4944,7 +5198,92 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4973,13 +5312,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color auto="1"/>
       </font>
@@ -4992,265 +5324,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5288,22 +5362,17 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <color auto="1"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5335,24 +5404,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5421,48 +5472,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5474,9 +5484,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5512,33 +5525,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5555,31 +5544,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5617,7 +5582,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5634,7 +5599,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5642,44 +5607,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5703,7 +5630,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5717,7 +5644,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5766,9 +5693,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5806,7 +5733,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5912,7 +5839,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6054,7 +5981,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6064,8 +5991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O822"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A406" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A413" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B406" sqref="B406"/>
     </sheetView>
   </sheetViews>
@@ -30132,17 +30059,17 @@
     </sortState>
   </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="G404 I1:I1048576">
-    <cfRule type="cellIs" dxfId="119" priority="1" operator="equal">
+  <conditionalFormatting sqref="I1:I1048576 G404">
+    <cfRule type="cellIs" dxfId="107" priority="1" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="2" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="3" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="4" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30153,11 +30080,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F04922E-3981-41FC-85A3-60DC4C62ADCB}">
-  <dimension ref="A1:N284"/>
+  <dimension ref="A1:N285"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A279" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L284" sqref="L284"/>
+      <selection pane="bottomLeft" activeCell="N286" sqref="N286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40584,7 +40511,7 @@
         <v>5772097</v>
       </c>
     </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A273" s="22">
         <v>45784</v>
       </c>
@@ -40613,7 +40540,7 @@
         <v>462529</v>
       </c>
     </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A274" s="22">
         <v>45785</v>
       </c>
@@ -40642,7 +40569,7 @@
         <v>5773009</v>
       </c>
     </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A275" s="22">
         <v>45878</v>
       </c>
@@ -40668,7 +40595,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A276" s="22">
         <v>45878</v>
       </c>
@@ -40694,7 +40621,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A277" s="22">
         <v>45786</v>
       </c>
@@ -40720,7 +40647,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A278" s="22">
         <v>45786</v>
       </c>
@@ -40749,7 +40676,7 @@
         <v>5774734</v>
       </c>
     </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A279" s="22">
         <v>45786</v>
       </c>
@@ -40778,7 +40705,7 @@
         <v>5774778</v>
       </c>
     </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A280" s="22">
         <v>45789</v>
       </c>
@@ -40804,7 +40731,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A281" s="22">
         <v>45789</v>
       </c>
@@ -40830,7 +40757,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A282" s="22">
         <v>45789</v>
       </c>
@@ -40856,7 +40783,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A283" s="22">
         <v>45789</v>
       </c>
@@ -40885,7 +40812,7 @@
         <v>462666</v>
       </c>
     </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A284" s="22">
         <v>45790</v>
       </c>
@@ -40912,6 +40839,38 @@
       </c>
       <c r="L284" s="2">
         <v>462706</v>
+      </c>
+    </row>
+    <row r="285" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A285" s="22">
+        <v>45791</v>
+      </c>
+      <c r="B285" s="7" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C285" s="7" t="s">
+        <v>1476</v>
+      </c>
+      <c r="D285" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E285" s="3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="F285" s="25">
+        <v>200</v>
+      </c>
+      <c r="H285" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="J285" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L285" s="2">
+        <v>111111</v>
+      </c>
+      <c r="N285" s="2" t="s">
+        <v>1478</v>
       </c>
     </row>
   </sheetData>
@@ -40921,425 +40880,387 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="I1:I144">
-    <cfRule type="cellIs" dxfId="115" priority="280" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="282" operator="equal">
+      <formula>"NEGADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="102" priority="281" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="280" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="281" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="282" operator="equal">
-      <formula>"NEGADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="283" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="283" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="expression" dxfId="111" priority="119">
+    <cfRule type="expression" dxfId="99" priority="119">
       <formula>"NEGAGO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I146">
-    <cfRule type="cellIs" dxfId="110" priority="276" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="277" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="97" priority="276" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="277" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
+    <cfRule type="cellIs" dxfId="96" priority="279" operator="equal">
+      <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="278" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="278" operator="equal">
       <formula>"NEGADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="279" operator="equal">
-      <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I148:I190">
-    <cfRule type="cellIs" dxfId="106" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="145" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="147" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="145" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="146" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="144" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I192:I193">
-    <cfRule type="cellIs" dxfId="102" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="148" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="151" operator="equal">
+      <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="149" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="151" operator="equal">
-      <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I192:I195">
-    <cfRule type="cellIs" dxfId="99" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="99" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I194:I195">
-    <cfRule type="cellIs" dxfId="98" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="97" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="98" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="100" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I195">
-    <cfRule type="cellIs" dxfId="95" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="171" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="169" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="169" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="168" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I198:I200">
-    <cfRule type="cellIs" dxfId="92" priority="164" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="166" operator="equal">
+      <formula>"NEGADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="79" priority="167" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="165" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="164" operator="equal">
+      <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="77" priority="165" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="166" operator="equal">
-      <formula>"NEGADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="167" operator="equal">
-      <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I202:I203">
-    <cfRule type="cellIs" dxfId="88" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="71" operator="equal">
+      <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="75" priority="68" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="69" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="70" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="71" operator="equal">
-      <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I205:I206">
-    <cfRule type="cellIs" dxfId="84" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="86" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="87" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="88" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="89" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I206">
-    <cfRule type="cellIs" dxfId="80" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="96" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="94" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I208:I211">
-    <cfRule type="cellIs" dxfId="78" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="117" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="115" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="116" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="114" operator="equal">
       <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="115" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I213:I214">
-    <cfRule type="cellIs" dxfId="74" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="124" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="127" operator="equal">
+      <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="125" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="127" operator="equal">
-      <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I213:I215">
-    <cfRule type="cellIs" dxfId="71" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="112" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I215">
-    <cfRule type="cellIs" dxfId="70" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="113" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="111" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="110" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I216">
-    <cfRule type="expression" dxfId="67" priority="118">
+    <cfRule type="expression" dxfId="55" priority="118">
       <formula>"NEGADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I217:I220">
-    <cfRule type="cellIs" dxfId="66" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="132" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="135" operator="equal">
+      <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="133" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="134" operator="equal">
       <formula>"NEGADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="135" operator="equal">
-      <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I221">
-    <cfRule type="expression" dxfId="62" priority="105">
+    <cfRule type="expression" dxfId="50" priority="105">
       <formula>"NEGADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I222:I223">
-    <cfRule type="cellIs" dxfId="61" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="102" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="104" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="102" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="101" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I222:I229">
-    <cfRule type="cellIs" dxfId="58" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="74" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I224">
-    <cfRule type="cellIs" dxfId="57" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="121" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="120" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="121" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="123" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I225:I229">
-    <cfRule type="cellIs" dxfId="54" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="73" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="75" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="73" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="72" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I226:I229">
-    <cfRule type="expression" dxfId="51" priority="76">
+    <cfRule type="expression" dxfId="39" priority="76">
       <formula>"NEGADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I231:I232">
-    <cfRule type="cellIs" dxfId="50" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="129" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="128" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="129" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="130" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="131" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I234">
-    <cfRule type="cellIs" dxfId="46" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="136" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="137" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="138" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="139" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I236:I237">
-    <cfRule type="cellIs" dxfId="42" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
+      <formula>"NEGADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="29" operator="equal">
-      <formula>"NEGADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I239:I244">
-    <cfRule type="cellIs" dxfId="38" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="33" operator="equal">
+      <formula>"NEGADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="32" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="31" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="32" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="33" operator="equal">
-      <formula>"NEGADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="34" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I242:I243">
-    <cfRule type="expression" dxfId="34" priority="35">
+    <cfRule type="expression" dxfId="22" priority="35">
       <formula>"NEGADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I247">
-    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
+      <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
+      <formula>"NEGADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="7" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I250">
+    <cfRule type="expression" dxfId="17" priority="13">
       <formula>"NEGADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="8" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I250:I256">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+      <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+      <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+      <formula>"NEGADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I258">
+    <cfRule type="cellIs" dxfId="12" priority="51" operator="equal">
+      <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="50" operator="equal">
+      <formula>"NEGADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="49" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="48" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I250">
-    <cfRule type="cellIs" dxfId="29" priority="9" operator="equal">
+  <conditionalFormatting sqref="I260:I265">
+    <cfRule type="cellIs" dxfId="8" priority="15" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="17" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="10" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="16" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="12" operator="equal">
-      <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="13">
-      <formula>"NEGADO"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I253:I256">
-    <cfRule type="cellIs" dxfId="24" priority="40" operator="equal">
-      <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="41" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="42" operator="equal">
-      <formula>"NEGADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="43" operator="equal">
-      <formula>"LIQUIDADO"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I258">
-    <cfRule type="cellIs" dxfId="20" priority="48" operator="equal">
-      <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="49" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="50" operator="equal">
-      <formula>"NEGADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="51" operator="equal">
-      <formula>"LIQUIDADO"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I260:I263">
-    <cfRule type="cellIs" dxfId="16" priority="23" operator="equal">
-      <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="24" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="25" operator="equal">
-      <formula>"NEGADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="14" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I264:I265">
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
-      <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
-      <formula>"NEGADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
-      <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="18">
+    <cfRule type="expression" dxfId="4" priority="18">
       <formula>"NEGADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I267">
-    <cfRule type="cellIs" dxfId="7" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="20" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="19" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="20" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="21" operator="equal">
-      <formula>"NEGADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="22" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I251:I252">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="21" operator="equal">
       <formula>"NEGADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
-      <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualización automática: 2025-06-22 22:07:20.338495
</commit_message>
<xml_diff>
--- a/CONTROL REEMBOLSOS.xlsx
+++ b/CONTROL REEMBOLSOS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seidor.ANALYTICS-EC001\Downloads\TRABAJOS_EXTRAS\TESIS_RUTH_AXEL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE43FAE0-59FF-4310-8D5C-7EAF5620D551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4859B374-5B0C-465A-961D-FCB27ADE7001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3885" yWindow="3885" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REEMBOLSOS 2024" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -42,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6149" uniqueCount="1479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6156" uniqueCount="1482">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -4479,6 +4477,15 @@
   </si>
   <si>
     <t>esto es un test de actualizacion</t>
+  </si>
+  <si>
+    <t>AXEL GALVES</t>
+  </si>
+  <si>
+    <t>AAXEL GALVES</t>
+  </si>
+  <si>
+    <t>PENDIENTE DE FACTURA</t>
   </si>
 </sst>
 </file>
@@ -4486,8 +4493,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;\-#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="_ &quot;$&quot;* #,##0.00_ ;_ &quot;$&quot;* \-#,##0.00_ ;_ &quot;$&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;\-#,##0.00"/>
+    <numFmt numFmtId="44" formatCode="_ &quot;$&quot;* #,##0.00_ ;_ &quot;$&quot;* \-#,##0.00_ ;_ &quot;$&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -4712,7 +4719,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -4779,13 +4786,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4809,13 +4816,13 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="12" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="12" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5693,9 +5700,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5733,7 +5740,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5839,7 +5846,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5981,7 +5988,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -30080,11 +30087,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F04922E-3981-41FC-85A3-60DC4C62ADCB}">
-  <dimension ref="A1:N285"/>
+  <dimension ref="A1:N286"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A279" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N286" sqref="N286"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A273" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N287" sqref="N287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40871,6 +40878,35 @@
       </c>
       <c r="N285" s="2" t="s">
         <v>1478</v>
+      </c>
+    </row>
+    <row r="286" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A286" s="22">
+        <v>45830</v>
+      </c>
+      <c r="B286" s="7" t="s">
+        <v>1479</v>
+      </c>
+      <c r="C286" s="2" t="s">
+        <v>1480</v>
+      </c>
+      <c r="D286" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E286" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="F286" s="25">
+        <v>150</v>
+      </c>
+      <c r="H286" s="3" t="s">
+        <v>1479</v>
+      </c>
+      <c r="J286" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N286" s="2" t="s">
+        <v>1481</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática: 2025-06-23 18:21:58.295878
</commit_message>
<xml_diff>
--- a/CONTROL REEMBOLSOS.xlsx
+++ b/CONTROL REEMBOLSOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC6356B-1F3F-40F4-9719-A8338C63F6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E54E5E-0224-4EBC-A586-B477605EE65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6163" uniqueCount="1484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6164" uniqueCount="1484">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -30096,8 +30096,8 @@
   <dimension ref="A1:N287"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N288" sqref="N288"/>
+      <pane ySplit="1" topLeftCell="A279" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I287" sqref="I287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -40936,6 +40936,9 @@
       </c>
       <c r="H287" s="3" t="s">
         <v>12</v>
+      </c>
+      <c r="I287" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="J287" s="3" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Actualización automática: 2025-06-23 18:52:11.213249
</commit_message>
<xml_diff>
--- a/CONTROL REEMBOLSOS.xlsx
+++ b/CONTROL REEMBOLSOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E54E5E-0224-4EBC-A586-B477605EE65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB29130-078F-4145-9413-CBA45064FFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6164" uniqueCount="1484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6171" uniqueCount="1484">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -30093,11 +30093,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F04922E-3981-41FC-85A3-60DC4C62ADCB}">
-  <dimension ref="A1:N287"/>
+  <dimension ref="A1:N288"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A279" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I287" sqref="I287"/>
+      <pane ySplit="1" topLeftCell="A278" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N288" sqref="N288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -40948,6 +40948,41 @@
       </c>
       <c r="N287" s="2" t="s">
         <v>1483</v>
+      </c>
+    </row>
+    <row r="288" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A288" s="22">
+        <v>45831</v>
+      </c>
+      <c r="B288" s="7" t="s">
+        <v>1475</v>
+      </c>
+      <c r="C288" s="2" t="s">
+        <v>1475</v>
+      </c>
+      <c r="D288" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E288" s="3" t="s">
+        <v>950</v>
+      </c>
+      <c r="F288" s="25">
+        <v>50</v>
+      </c>
+      <c r="G288" s="26">
+        <v>25</v>
+      </c>
+      <c r="H288" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I288" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J288" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L288" s="2">
+        <v>412412</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática: 2025-06-24 21:42:04.940057
</commit_message>
<xml_diff>
--- a/CONTROL REEMBOLSOS.xlsx
+++ b/CONTROL REEMBOLSOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB29130-078F-4145-9413-CBA45064FFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E731CE5-6A45-4C63-8801-0517FB504015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6171" uniqueCount="1484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6178" uniqueCount="1487">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -4492,6 +4492,15 @@
   </si>
   <si>
     <t>FALTA REGULARIZA FACTURA</t>
+  </si>
+  <si>
+    <t>RUTH GUZMAN</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>OTROTEST</t>
   </si>
 </sst>
 </file>
@@ -30093,11 +30102,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F04922E-3981-41FC-85A3-60DC4C62ADCB}">
-  <dimension ref="A1:N288"/>
+  <dimension ref="A1:N289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A278" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N288" sqref="N288"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A277" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O291" sqref="O291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -40983,6 +40992,38 @@
       </c>
       <c r="L288" s="2">
         <v>412412</v>
+      </c>
+    </row>
+    <row r="289" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A289" s="22">
+        <v>45832</v>
+      </c>
+      <c r="B289" s="7" t="s">
+        <v>1484</v>
+      </c>
+      <c r="C289" s="2" t="s">
+        <v>1484</v>
+      </c>
+      <c r="D289" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E289" s="3" t="s">
+        <v>1485</v>
+      </c>
+      <c r="F289" s="25">
+        <v>50</v>
+      </c>
+      <c r="H289" s="3" t="s">
+        <v>1479</v>
+      </c>
+      <c r="J289" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L289" s="2">
+        <v>110000</v>
+      </c>
+      <c r="N289" s="2" t="s">
+        <v>1486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática: 2025-06-24 22:21:53.526285
</commit_message>
<xml_diff>
--- a/CONTROL REEMBOLSOS.xlsx
+++ b/CONTROL REEMBOLSOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E731CE5-6A45-4C63-8801-0517FB504015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE0CD0C-29FA-481C-B0C7-8104AA62BA04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6178" uniqueCount="1487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6186" uniqueCount="1490">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -4501,6 +4501,15 @@
   </si>
   <si>
     <t>OTROTEST</t>
+  </si>
+  <si>
+    <t>LUISA GUZMAN</t>
+  </si>
+  <si>
+    <t>TEST 2</t>
+  </si>
+  <si>
+    <t>OTROTEST2</t>
   </si>
 </sst>
 </file>
@@ -30102,11 +30111,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F04922E-3981-41FC-85A3-60DC4C62ADCB}">
-  <dimension ref="A1:N289"/>
+  <dimension ref="A1:N290"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A277" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O291" sqref="O291"/>
+      <selection pane="bottomLeft" activeCell="N291" sqref="N291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -41024,6 +41033,44 @@
       </c>
       <c r="N289" s="2" t="s">
         <v>1486</v>
+      </c>
+    </row>
+    <row r="290" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A290" s="22">
+        <v>45832</v>
+      </c>
+      <c r="B290" s="7" t="s">
+        <v>1487</v>
+      </c>
+      <c r="C290" s="2" t="s">
+        <v>1487</v>
+      </c>
+      <c r="D290" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E290" s="3" t="s">
+        <v>1488</v>
+      </c>
+      <c r="F290" s="25">
+        <v>50</v>
+      </c>
+      <c r="G290" s="26">
+        <v>10</v>
+      </c>
+      <c r="H290" s="3" t="s">
+        <v>1479</v>
+      </c>
+      <c r="I290" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J290" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L290" s="2">
+        <v>110001</v>
+      </c>
+      <c r="N290" s="2" t="s">
+        <v>1489</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática: 2025-06-30 19:18:20.097018
</commit_message>
<xml_diff>
--- a/CONTROL REEMBOLSOS.xlsx
+++ b/CONTROL REEMBOLSOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE0CD0C-29FA-481C-B0C7-8104AA62BA04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BABD985-6512-4583-A50E-1C07433F650A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6186" uniqueCount="1490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6187" uniqueCount="1490">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -4470,15 +4470,6 @@
     <t>CARMEN SOTO</t>
   </si>
   <si>
-    <t>FREDDY QUIMIS</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>esto es un test de actualizacion</t>
-  </si>
-  <si>
     <t>AXEL GALVES</t>
   </si>
   <si>
@@ -4510,6 +4501,15 @@
   </si>
   <si>
     <t>OTROTEST2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JORGE GUZMAN </t>
+  </si>
+  <si>
+    <t>TEST3</t>
+  </si>
+  <si>
+    <t>OTROTEST3</t>
   </si>
 </sst>
 </file>
@@ -4868,13 +4868,6 @@
   </cellStyles>
   <dxfs count="108">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color auto="1"/>
       </font>
@@ -4887,46 +4880,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4945,166 +4899,10 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5159,22 +4957,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5182,139 +4965,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5343,6 +4993,21 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color auto="1"/>
       </font>
@@ -5355,7 +5020,195 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5393,17 +5246,22 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5435,6 +5293,24 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5503,7 +5379,48 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5515,12 +5432,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5556,9 +5470,33 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5575,7 +5513,31 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5613,7 +5575,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5630,7 +5592,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5638,6 +5600,44 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5661,7 +5661,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5675,7 +5675,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -40874,60 +40874,63 @@
     </row>
     <row r="285" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A285" s="22">
-        <v>45791</v>
+        <v>45830</v>
       </c>
       <c r="B285" s="7" t="s">
         <v>1476</v>
       </c>
-      <c r="C285" s="7" t="s">
+      <c r="C285" s="2" t="s">
         <v>1476</v>
       </c>
       <c r="D285" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E285" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="F285" s="25">
+        <v>150</v>
+      </c>
+      <c r="H285" s="3" t="s">
+        <v>1476</v>
+      </c>
+      <c r="J285" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N285" s="2" t="s">
         <v>1477</v>
-      </c>
-      <c r="F285" s="25">
-        <v>200</v>
-      </c>
-      <c r="H285" s="3" t="s">
-        <v>1026</v>
-      </c>
-      <c r="J285" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L285" s="2">
-        <v>111111</v>
-      </c>
-      <c r="N285" s="2" t="s">
-        <v>1478</v>
       </c>
     </row>
     <row r="286" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A286" s="22">
-        <v>45830</v>
+        <v>45831</v>
       </c>
       <c r="B286" s="7" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="C286" s="2" t="s">
         <v>1479</v>
       </c>
       <c r="D286" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E286" s="3" t="s">
-        <v>756</v>
+        <v>997</v>
       </c>
       <c r="F286" s="25">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="H286" s="3" t="s">
-        <v>1479</v>
+        <v>12</v>
+      </c>
+      <c r="I286" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="J286" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="L286" s="2">
+        <v>4212442</v>
       </c>
       <c r="N286" s="2" t="s">
         <v>1480</v>
@@ -40938,22 +40941,25 @@
         <v>45831</v>
       </c>
       <c r="B287" s="7" t="s">
-        <v>1481</v>
+        <v>1475</v>
       </c>
       <c r="C287" s="2" t="s">
-        <v>1482</v>
+        <v>1475</v>
       </c>
       <c r="D287" s="3" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E287" s="3" t="s">
-        <v>997</v>
+        <v>950</v>
       </c>
       <c r="F287" s="25">
-        <v>300</v>
+        <v>50</v>
+      </c>
+      <c r="G287" s="26">
+        <v>25</v>
       </c>
       <c r="H287" s="3" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="I287" s="3" t="s">
         <v>7</v>
@@ -40962,45 +40968,39 @@
         <v>8</v>
       </c>
       <c r="L287" s="2">
-        <v>4212442</v>
-      </c>
-      <c r="N287" s="2" t="s">
-        <v>1483</v>
+        <v>412412</v>
       </c>
     </row>
     <row r="288" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A288" s="22">
-        <v>45831</v>
+        <v>45832</v>
       </c>
       <c r="B288" s="7" t="s">
-        <v>1475</v>
+        <v>1481</v>
       </c>
       <c r="C288" s="2" t="s">
-        <v>1475</v>
+        <v>1481</v>
       </c>
       <c r="D288" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E288" s="3" t="s">
-        <v>950</v>
+        <v>1482</v>
       </c>
       <c r="F288" s="25">
         <v>50</v>
       </c>
-      <c r="G288" s="26">
-        <v>25</v>
-      </c>
       <c r="H288" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I288" s="3" t="s">
-        <v>7</v>
+        <v>1476</v>
       </c>
       <c r="J288" s="3" t="s">
         <v>8</v>
       </c>
       <c r="L288" s="2">
-        <v>412412</v>
+        <v>110000</v>
+      </c>
+      <c r="N288" s="2" t="s">
+        <v>1483</v>
       </c>
     </row>
     <row r="289" spans="1:14" x14ac:dyDescent="0.35">
@@ -41022,14 +41022,20 @@
       <c r="F289" s="25">
         <v>50</v>
       </c>
+      <c r="G289" s="26">
+        <v>10</v>
+      </c>
       <c r="H289" s="3" t="s">
-        <v>1479</v>
+        <v>1476</v>
+      </c>
+      <c r="I289" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="J289" s="3" t="s">
         <v>8</v>
       </c>
       <c r="L289" s="2">
-        <v>110000</v>
+        <v>110001</v>
       </c>
       <c r="N289" s="2" t="s">
         <v>1486</v>
@@ -41037,7 +41043,7 @@
     </row>
     <row r="290" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A290" s="22">
-        <v>45832</v>
+        <v>45838</v>
       </c>
       <c r="B290" s="7" t="s">
         <v>1487</v>
@@ -41046,19 +41052,19 @@
         <v>1487</v>
       </c>
       <c r="D290" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E290" s="3" t="s">
         <v>1488</v>
       </c>
       <c r="F290" s="25">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G290" s="26">
         <v>10</v>
       </c>
       <c r="H290" s="3" t="s">
-        <v>1479</v>
+        <v>1476</v>
       </c>
       <c r="I290" s="3" t="s">
         <v>7</v>
@@ -41067,7 +41073,7 @@
         <v>8</v>
       </c>
       <c r="L290" s="2">
-        <v>110001</v>
+        <v>170001</v>
       </c>
       <c r="N290" s="2" t="s">
         <v>1489</v>
@@ -41080,14 +41086,14 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="I1:I144">
-    <cfRule type="cellIs" dxfId="103" priority="282" operator="equal">
-      <formula>"NEGADO"</formula>
+    <cfRule type="cellIs" dxfId="103" priority="280" operator="equal">
+      <formula>"LIQUIDADO"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="102" priority="281" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="280" operator="equal">
-      <formula>"LIQUIDADO"</formula>
+    <cfRule type="cellIs" dxfId="101" priority="282" operator="equal">
+      <formula>"NEGADO"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="100" priority="283" operator="equal">
       <formula>"LIQUIDADO"</formula>
@@ -41099,30 +41105,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I146">
-    <cfRule type="cellIs" dxfId="98" priority="277" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="276" operator="equal">
+      <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="97" priority="277" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="276" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="278" operator="equal">
+      <formula>"NEGADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="279" operator="equal">
       <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="279" operator="equal">
-      <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="278" operator="equal">
-      <formula>"NEGADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I148:I190">
-    <cfRule type="cellIs" dxfId="94" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="144" operator="equal">
+      <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="145" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="147" operator="equal">
-      <formula>"LIQUIDADO"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="92" priority="146" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="147" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41130,11 +41136,11 @@
     <cfRule type="cellIs" dxfId="90" priority="148" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="151" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="149" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="151" operator="equal">
       <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="149" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I192:I195">
@@ -41154,42 +41160,42 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I195">
-    <cfRule type="cellIs" dxfId="83" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="168" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="82" priority="169" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="171" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I198:I200">
-    <cfRule type="cellIs" dxfId="80" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="164" operator="equal">
+      <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="79" priority="165" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="166" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="167" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="167" operator="equal">
       <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="164" operator="equal">
-      <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="165" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I202:I203">
-    <cfRule type="cellIs" dxfId="76" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="68" operator="equal">
+      <formula>"NEGADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="75" priority="69" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="68" operator="equal">
-      <formula>"NEGADO"</formula>
+    <cfRule type="cellIs" dxfId="74" priority="70" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="71" operator="equal">
       <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="70" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I205:I206">
@@ -41207,36 +41213,36 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I206">
-    <cfRule type="cellIs" dxfId="68" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="94" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="96" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I208:I211">
-    <cfRule type="cellIs" dxfId="66" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="114" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="115" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="116" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="117" operator="equal">
       <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="115" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I213:I214">
     <cfRule type="cellIs" dxfId="62" priority="124" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="125" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="127" operator="equal">
       <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="125" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I213:I215">
@@ -41245,13 +41251,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I215">
-    <cfRule type="cellIs" dxfId="58" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="110" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="57" priority="111" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="113" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41264,14 +41270,14 @@
     <cfRule type="cellIs" dxfId="54" priority="132" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="135" operator="equal">
-      <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="133" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="134" operator="equal">
       <formula>"NEGADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="135" operator="equal">
+      <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I221">
@@ -41280,13 +41286,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I222:I223">
-    <cfRule type="cellIs" dxfId="49" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="101" operator="equal">
+      <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="102" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="104" operator="equal">
-      <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="104" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41296,24 +41302,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I224">
-    <cfRule type="cellIs" dxfId="45" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="120" operator="equal">
+      <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="121" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="120" operator="equal">
-      <formula>"LIQUIDADO"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="43" priority="123" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I225:I229">
-    <cfRule type="cellIs" dxfId="42" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="72" operator="equal">
+      <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="73" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="75" operator="equal">
-      <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="75" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41323,11 +41329,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I231:I232">
-    <cfRule type="cellIs" dxfId="38" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="128" operator="equal">
+      <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="129" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="128" operator="equal">
-      <formula>"LIQUIDADO"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="36" priority="130" operator="equal">
       <formula>"NEGADO"</formula>
@@ -41351,28 +41357,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I236:I237">
-    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="27" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I239:I244">
-    <cfRule type="cellIs" dxfId="26" priority="33" operator="equal">
-      <formula>"NEGADO"</formula>
+    <cfRule type="cellIs" dxfId="26" priority="31" operator="equal">
+      <formula>"LIQUIDADO"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="25" priority="32" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="31" operator="equal">
-      <formula>"LIQUIDADO"</formula>
+    <cfRule type="cellIs" dxfId="24" priority="33" operator="equal">
+      <formula>"NEGADO"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="23" priority="34" operator="equal">
       <formula>"LIQUIDADO"</formula>
@@ -41387,14 +41393,14 @@
     <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
-      <formula>"LIQUIDADO"</formula>
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
+    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+      <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I250">
@@ -41406,41 +41412,41 @@
     <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
-      <formula>"LIQUIDADO"</formula>
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
+      <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I258">
-    <cfRule type="cellIs" dxfId="12" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="48" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="49" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="50" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="49" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="51" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I260:I265">
-    <cfRule type="cellIs" dxfId="8" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="14" operator="equal">
+      <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="15" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="17" operator="equal">
-      <formula>"LIQUIDADO"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="16" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="17" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41450,17 +41456,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I267">
-    <cfRule type="cellIs" dxfId="3" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="19" operator="equal">
+      <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="20" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="21" operator="equal">
+      <formula>"NEGADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="22" operator="equal">
       <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="22" operator="equal">
-      <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="21" operator="equal">
-      <formula>"NEGADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualización automática: 2025-07-08 20:42:49.231447
</commit_message>
<xml_diff>
--- a/CONTROL REEMBOLSOS.xlsx
+++ b/CONTROL REEMBOLSOS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BABD985-6512-4583-A50E-1C07433F650A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83E2E69-D31B-4748-99CF-6BA83C884508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6187" uniqueCount="1490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6194" uniqueCount="1493">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -4510,6 +4510,15 @@
   </si>
   <si>
     <t>OTROTEST3</t>
+  </si>
+  <si>
+    <t>LUISITO COMUNICA</t>
+  </si>
+  <si>
+    <t>TEST4</t>
+  </si>
+  <si>
+    <t>OTROTEST4</t>
   </si>
 </sst>
 </file>
@@ -4868,6 +4877,13 @@
   </cellStyles>
   <dxfs count="108">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color auto="1"/>
       </font>
@@ -4880,7 +4896,46 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4899,10 +4954,166 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4957,6 +5168,69 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -4964,7 +5238,92 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4993,21 +5352,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color auto="1"/>
       </font>
@@ -5020,195 +5364,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5246,22 +5402,17 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <color auto="1"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5293,24 +5444,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5379,48 +5512,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5432,9 +5524,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5470,33 +5565,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5513,31 +5584,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5575,7 +5622,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5592,7 +5639,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5600,44 +5647,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5661,7 +5670,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5675,7 +5684,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -30111,10 +30120,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F04922E-3981-41FC-85A3-60DC4C62ADCB}">
-  <dimension ref="A1:N290"/>
+  <dimension ref="A1:N291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A277" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A280" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N291" sqref="N291"/>
     </sheetView>
   </sheetViews>
@@ -41079,6 +41088,41 @@
         <v>1489</v>
       </c>
     </row>
+    <row r="291" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A291" s="22">
+        <v>45846</v>
+      </c>
+      <c r="B291" s="7" t="s">
+        <v>1490</v>
+      </c>
+      <c r="C291" s="2" t="s">
+        <v>1490</v>
+      </c>
+      <c r="D291" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E291" s="3" t="s">
+        <v>1491</v>
+      </c>
+      <c r="F291" s="25">
+        <v>60</v>
+      </c>
+      <c r="G291" s="26">
+        <v>50</v>
+      </c>
+      <c r="H291" s="3" t="s">
+        <v>1481</v>
+      </c>
+      <c r="J291" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L291" s="2">
+        <v>180001</v>
+      </c>
+      <c r="N291" s="2" t="s">
+        <v>1492</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:N283" xr:uid="{0F04922E-3981-41FC-85A3-60DC4C62ADCB}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N156">
@@ -41086,14 +41130,14 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="I1:I144">
-    <cfRule type="cellIs" dxfId="103" priority="280" operator="equal">
-      <formula>"LIQUIDADO"</formula>
+    <cfRule type="cellIs" dxfId="103" priority="282" operator="equal">
+      <formula>"NEGADO"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="102" priority="281" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="282" operator="equal">
-      <formula>"NEGADO"</formula>
+    <cfRule type="cellIs" dxfId="101" priority="280" operator="equal">
+      <formula>"LIQUIDADO"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="100" priority="283" operator="equal">
       <formula>"LIQUIDADO"</formula>
@@ -41105,30 +41149,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I146">
-    <cfRule type="cellIs" dxfId="98" priority="276" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="277" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="97" priority="276" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="277" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
+    <cfRule type="cellIs" dxfId="96" priority="279" operator="equal">
+      <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="278" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="278" operator="equal">
       <formula>"NEGADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="279" operator="equal">
-      <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I148:I190">
-    <cfRule type="cellIs" dxfId="94" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="145" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="147" operator="equal">
       <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="145" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="92" priority="146" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="144" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41136,11 +41180,11 @@
     <cfRule type="cellIs" dxfId="90" priority="148" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="151" operator="equal">
+      <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="149" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="151" operator="equal">
-      <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I192:I195">
@@ -41160,42 +41204,42 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I195">
-    <cfRule type="cellIs" dxfId="83" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="171" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="82" priority="169" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="168" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I198:I200">
-    <cfRule type="cellIs" dxfId="80" priority="164" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="166" operator="equal">
+      <formula>"NEGADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="79" priority="167" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="165" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="164" operator="equal">
+      <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="77" priority="165" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="166" operator="equal">
-      <formula>"NEGADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="167" operator="equal">
-      <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I202:I203">
-    <cfRule type="cellIs" dxfId="76" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="71" operator="equal">
+      <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="75" priority="68" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="69" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="70" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="71" operator="equal">
-      <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I205:I206">
@@ -41213,36 +41257,36 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I206">
-    <cfRule type="cellIs" dxfId="68" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="96" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="94" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I208:I211">
-    <cfRule type="cellIs" dxfId="66" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="117" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="115" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="116" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="114" operator="equal">
       <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="115" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I213:I214">
     <cfRule type="cellIs" dxfId="62" priority="124" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="127" operator="equal">
+      <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="125" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="127" operator="equal">
-      <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I213:I215">
@@ -41251,13 +41295,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I215">
-    <cfRule type="cellIs" dxfId="58" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="113" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="57" priority="111" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="110" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41270,14 +41314,14 @@
     <cfRule type="cellIs" dxfId="54" priority="132" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="135" operator="equal">
+      <formula>"LIQUIDADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="133" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="134" operator="equal">
       <formula>"NEGADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="135" operator="equal">
-      <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I221">
@@ -41286,13 +41330,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I222:I223">
-    <cfRule type="cellIs" dxfId="49" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="102" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="104" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="102" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="101" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41302,24 +41346,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I224">
-    <cfRule type="cellIs" dxfId="45" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="121" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="120" operator="equal">
       <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="121" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="43" priority="123" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I225:I229">
-    <cfRule type="cellIs" dxfId="42" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="73" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="75" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="73" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="72" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41329,11 +41373,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I231:I232">
-    <cfRule type="cellIs" dxfId="38" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="129" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="128" operator="equal">
       <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="129" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="36" priority="130" operator="equal">
       <formula>"NEGADO"</formula>
@@ -41357,28 +41401,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I236:I237">
-    <cfRule type="cellIs" dxfId="30" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
+      <formula>"NEGADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
-      <formula>"NEGADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I239:I244">
-    <cfRule type="cellIs" dxfId="26" priority="31" operator="equal">
-      <formula>"LIQUIDADO"</formula>
+    <cfRule type="cellIs" dxfId="26" priority="33" operator="equal">
+      <formula>"NEGADO"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="25" priority="32" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="33" operator="equal">
-      <formula>"NEGADO"</formula>
+    <cfRule type="cellIs" dxfId="24" priority="31" operator="equal">
+      <formula>"LIQUIDADO"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="23" priority="34" operator="equal">
       <formula>"LIQUIDADO"</formula>
@@ -41393,14 +41437,14 @@
     <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
+    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
+      <formula>"LIQUIDADO"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
-      <formula>"LIQUIDADO"</formula>
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I250">
@@ -41412,41 +41456,41 @@
     <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+      <formula>"LIQUIDADO"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
-      <formula>"LIQUIDADO"</formula>
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I258">
-    <cfRule type="cellIs" dxfId="12" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="51" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="50" operator="equal">
+      <formula>"NEGADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="49" operator="equal">
       <formula>"INFO ADICIONAL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="50" operator="equal">
-      <formula>"NEGADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="48" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I260:I265">
-    <cfRule type="cellIs" dxfId="8" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="15" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="17" operator="equal">
       <formula>"LIQUIDADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="15" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="16" operator="equal">
       <formula>"NEGADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="14" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41456,17 +41500,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I267">
-    <cfRule type="cellIs" dxfId="3" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="20" operator="equal">
+      <formula>"INFO ADICIONAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="19" operator="equal">
       <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="20" operator="equal">
-      <formula>"INFO ADICIONAL"</formula>
+    <cfRule type="cellIs" dxfId="1" priority="22" operator="equal">
+      <formula>"LIQUIDADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="21" operator="equal">
       <formula>"NEGADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="22" operator="equal">
-      <formula>"LIQUIDADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualización automática: 2025-08-16 13:34:34.921322
</commit_message>
<xml_diff>
--- a/CONTROL REEMBOLSOS.xlsx
+++ b/CONTROL REEMBOLSOS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83E2E69-D31B-4748-99CF-6BA83C884508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD17D0D-0540-419E-83F0-AA98D4A7A2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6194" uniqueCount="1493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6201" uniqueCount="1496">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -4519,6 +4519,15 @@
   </si>
   <si>
     <t>OTROTEST4</t>
+  </si>
+  <si>
+    <t>FIBRE</t>
+  </si>
+  <si>
+    <t>AXEL GAÑVES</t>
+  </si>
+  <si>
+    <t>A la espera de dcumentacion</t>
   </si>
 </sst>
 </file>
@@ -30120,11 +30129,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F04922E-3981-41FC-85A3-60DC4C62ADCB}">
-  <dimension ref="A1:N291"/>
+  <dimension ref="A1:N292"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A280" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N291" sqref="N291"/>
+      <selection pane="bottomLeft" activeCell="N293" sqref="N293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -41121,6 +41130,38 @@
       </c>
       <c r="N291" s="2" t="s">
         <v>1492</v>
+      </c>
+    </row>
+    <row r="292" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A292" s="22">
+        <v>45885</v>
+      </c>
+      <c r="B292" s="7" t="s">
+        <v>1481</v>
+      </c>
+      <c r="C292" s="2" t="s">
+        <v>1481</v>
+      </c>
+      <c r="D292" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E292" s="3" t="s">
+        <v>1493</v>
+      </c>
+      <c r="F292" s="25">
+        <v>200</v>
+      </c>
+      <c r="H292" s="3" t="s">
+        <v>1494</v>
+      </c>
+      <c r="J292" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L292" s="2">
+        <v>19900</v>
+      </c>
+      <c r="N292" s="2" t="s">
+        <v>1495</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática: 2025-08-16 13:43:17.514348
</commit_message>
<xml_diff>
--- a/CONTROL REEMBOLSOS.xlsx
+++ b/CONTROL REEMBOLSOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD17D0D-0540-419E-83F0-AA98D4A7A2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6862E8DF-8F06-4734-8D5B-6CA9425BA1B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6201" uniqueCount="1496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6201" uniqueCount="1495">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -4522,9 +4522,6 @@
   </si>
   <si>
     <t>FIBRE</t>
-  </si>
-  <si>
-    <t>AXEL GAÑVES</t>
   </si>
   <si>
     <t>A la espera de dcumentacion</t>
@@ -30133,7 +30130,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A280" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N293" sqref="N293"/>
+      <selection pane="bottomLeft" activeCell="H293" sqref="H293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -41152,7 +41149,7 @@
         <v>200</v>
       </c>
       <c r="H292" s="3" t="s">
-        <v>1494</v>
+        <v>1476</v>
       </c>
       <c r="J292" s="3" t="s">
         <v>8</v>
@@ -41161,7 +41158,7 @@
         <v>19900</v>
       </c>
       <c r="N292" s="2" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática: 2025-08-16 13:45:46.049466
</commit_message>
<xml_diff>
--- a/CONTROL REEMBOLSOS.xlsx
+++ b/CONTROL REEMBOLSOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6862E8DF-8F06-4734-8D5B-6CA9425BA1B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC29426-C76A-435F-9E29-2B4F7DFB871C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6201" uniqueCount="1495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6201" uniqueCount="1494">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -4519,9 +4519,6 @@
   </si>
   <si>
     <t>OTROTEST4</t>
-  </si>
-  <si>
-    <t>FIBRE</t>
   </si>
   <si>
     <t>A la espera de dcumentacion</t>
@@ -6038,8 +6035,8 @@
   <dimension ref="A1:O822"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A413" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B406" sqref="B406"/>
+      <pane ySplit="1" topLeftCell="A364" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C406" sqref="C406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -30128,9 +30125,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F04922E-3981-41FC-85A3-60DC4C62ADCB}">
   <dimension ref="A1:N292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A280" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H293" sqref="H293"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A277" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E293" sqref="E293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -40617,7 +40614,7 @@
     </row>
     <row r="275" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A275" s="22">
-        <v>45878</v>
+        <v>45786</v>
       </c>
       <c r="B275" s="7" t="s">
         <v>1466</v>
@@ -40643,7 +40640,7 @@
     </row>
     <row r="276" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A276" s="22">
-        <v>45878</v>
+        <v>45786</v>
       </c>
       <c r="B276" s="7" t="s">
         <v>1467</v>
@@ -41143,7 +41140,7 @@
         <v>20</v>
       </c>
       <c r="E292" s="3" t="s">
-        <v>1493</v>
+        <v>756</v>
       </c>
       <c r="F292" s="25">
         <v>200</v>
@@ -41158,7 +41155,7 @@
         <v>19900</v>
       </c>
       <c r="N292" s="2" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática: 2025-08-16 13:51:43.154332
</commit_message>
<xml_diff>
--- a/CONTROL REEMBOLSOS.xlsx
+++ b/CONTROL REEMBOLSOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC29426-C76A-435F-9E29-2B4F7DFB871C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F2574C-C958-4812-9DD2-970BD9963F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6201" uniqueCount="1494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6202" uniqueCount="1494">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -30125,9 +30125,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F04922E-3981-41FC-85A3-60DC4C62ADCB}">
   <dimension ref="A1:N292"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A277" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E293" sqref="E293"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A281" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M292" sqref="M292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -41148,11 +41148,17 @@
       <c r="H292" s="3" t="s">
         <v>1476</v>
       </c>
+      <c r="I292" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="J292" s="3" t="s">
         <v>8</v>
       </c>
       <c r="L292" s="2">
         <v>19900</v>
+      </c>
+      <c r="M292" s="6">
+        <v>45887</v>
       </c>
       <c r="N292" s="2" t="s">
         <v>1493</v>

</xml_diff>

<commit_message>
Actualización automática: 2025-08-16 16:23:28.829279
</commit_message>
<xml_diff>
--- a/CONTROL REEMBOLSOS.xlsx
+++ b/CONTROL REEMBOLSOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F2574C-C958-4812-9DD2-970BD9963F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EECBB55-B718-4A5E-B03B-2402207BC596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6202" uniqueCount="1494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6209" uniqueCount="1496">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -4522,6 +4522,12 @@
   </si>
   <si>
     <t>A la espera de dcumentacion</t>
+  </si>
+  <si>
+    <t>YADIRA DEL PINO</t>
+  </si>
+  <si>
+    <t>INFECCION</t>
   </si>
 </sst>
 </file>
@@ -30123,11 +30129,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F04922E-3981-41FC-85A3-60DC4C62ADCB}">
-  <dimension ref="A1:N292"/>
+  <dimension ref="A1:N293"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A281" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M292" sqref="M292"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A291" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O293" sqref="O293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -41114,7 +41120,7 @@
         <v>50</v>
       </c>
       <c r="H291" s="3" t="s">
-        <v>1481</v>
+        <v>1476</v>
       </c>
       <c r="J291" s="3" t="s">
         <v>8</v>
@@ -41161,6 +41167,38 @@
         <v>45887</v>
       </c>
       <c r="N292" s="2" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="293" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A293" s="22">
+        <v>45885</v>
+      </c>
+      <c r="B293" s="7" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C293" s="2" t="s">
+        <v>1494</v>
+      </c>
+      <c r="D293" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E293" s="3" t="s">
+        <v>1495</v>
+      </c>
+      <c r="F293" s="25">
+        <v>150</v>
+      </c>
+      <c r="H293" s="3" t="s">
+        <v>1476</v>
+      </c>
+      <c r="J293" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L293" s="2">
+        <v>2124</v>
+      </c>
+      <c r="N293" s="2" t="s">
         <v>1493</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática: 2025-08-16 16:41:22.675616
</commit_message>
<xml_diff>
--- a/CONTROL REEMBOLSOS.xlsx
+++ b/CONTROL REEMBOLSOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EECBB55-B718-4A5E-B03B-2402207BC596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D54C20-C314-4161-B7F8-7BCF2C03117E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30131,9 +30131,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F04922E-3981-41FC-85A3-60DC4C62ADCB}">
   <dimension ref="A1:N293"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A291" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O293" sqref="O293"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A290" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N293" sqref="N293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Actualización automática: 2025-08-17 22:23:30.701778
</commit_message>
<xml_diff>
--- a/CONTROL REEMBOLSOS.xlsx
+++ b/CONTROL REEMBOLSOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D54C20-C314-4161-B7F8-7BCF2C03117E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02E0885-2CD6-4CF7-8F28-4879308788C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6209" uniqueCount="1496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6216" uniqueCount="1496">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -30129,11 +30129,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F04922E-3981-41FC-85A3-60DC4C62ADCB}">
-  <dimension ref="A1:N293"/>
+  <dimension ref="A1:N294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A290" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N293" sqref="N293"/>
+      <selection pane="bottomLeft" activeCell="O294" sqref="O294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -41199,6 +41199,38 @@
         <v>2124</v>
       </c>
       <c r="N293" s="2" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="294" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A294" s="22">
+        <v>45886</v>
+      </c>
+      <c r="B294" s="7" t="s">
+        <v>1481</v>
+      </c>
+      <c r="C294" s="2" t="s">
+        <v>1481</v>
+      </c>
+      <c r="D294" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E294" s="3" t="s">
+        <v>774</v>
+      </c>
+      <c r="F294" s="25">
+        <v>300</v>
+      </c>
+      <c r="H294" s="3" t="s">
+        <v>1476</v>
+      </c>
+      <c r="J294" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L294" s="2">
+        <v>10021</v>
+      </c>
+      <c r="N294" s="2" t="s">
         <v>1493</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática: 2025-08-18 12:57:53.766979
</commit_message>
<xml_diff>
--- a/CONTROL REEMBOLSOS.xlsx
+++ b/CONTROL REEMBOLSOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02E0885-2CD6-4CF7-8F28-4879308788C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A92566-ADFB-4C79-95D0-473059160968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6216" uniqueCount="1496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6179" uniqueCount="1487">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -4501,33 +4501,6 @@
   </si>
   <si>
     <t>OTROTEST2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JORGE GUZMAN </t>
-  </si>
-  <si>
-    <t>TEST3</t>
-  </si>
-  <si>
-    <t>OTROTEST3</t>
-  </si>
-  <si>
-    <t>LUISITO COMUNICA</t>
-  </si>
-  <si>
-    <t>TEST4</t>
-  </si>
-  <si>
-    <t>OTROTEST4</t>
-  </si>
-  <si>
-    <t>A la espera de dcumentacion</t>
-  </si>
-  <si>
-    <t>YADIRA DEL PINO</t>
-  </si>
-  <si>
-    <t>INFECCION</t>
   </si>
 </sst>
 </file>
@@ -30132,8 +30105,8 @@
   <dimension ref="A1:N294"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A290" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O294" sqref="O294"/>
+      <pane ySplit="1" topLeftCell="A277" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I289" sqref="I289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -41060,179 +41033,20 @@
       </c>
     </row>
     <row r="290" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A290" s="22">
-        <v>45838</v>
-      </c>
-      <c r="B290" s="7" t="s">
-        <v>1487</v>
-      </c>
-      <c r="C290" s="2" t="s">
-        <v>1487</v>
-      </c>
-      <c r="D290" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E290" s="3" t="s">
-        <v>1488</v>
-      </c>
-      <c r="F290" s="25">
-        <v>40</v>
-      </c>
-      <c r="G290" s="26">
-        <v>10</v>
-      </c>
-      <c r="H290" s="3" t="s">
-        <v>1476</v>
-      </c>
-      <c r="I290" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J290" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L290" s="2">
-        <v>170001</v>
-      </c>
-      <c r="N290" s="2" t="s">
-        <v>1489</v>
-      </c>
+      <c r="A290" s="22"/>
     </row>
     <row r="291" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A291" s="22">
-        <v>45846</v>
-      </c>
-      <c r="B291" s="7" t="s">
-        <v>1490</v>
-      </c>
-      <c r="C291" s="2" t="s">
-        <v>1490</v>
-      </c>
-      <c r="D291" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E291" s="3" t="s">
-        <v>1491</v>
-      </c>
-      <c r="F291" s="25">
-        <v>60</v>
-      </c>
-      <c r="G291" s="26">
-        <v>50</v>
-      </c>
-      <c r="H291" s="3" t="s">
-        <v>1476</v>
-      </c>
-      <c r="J291" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L291" s="2">
-        <v>180001</v>
-      </c>
-      <c r="N291" s="2" t="s">
-        <v>1492</v>
-      </c>
+      <c r="A291" s="22"/>
     </row>
     <row r="292" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A292" s="22">
-        <v>45885</v>
-      </c>
-      <c r="B292" s="7" t="s">
-        <v>1481</v>
-      </c>
-      <c r="C292" s="2" t="s">
-        <v>1481</v>
-      </c>
-      <c r="D292" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E292" s="3" t="s">
-        <v>756</v>
-      </c>
-      <c r="F292" s="25">
-        <v>200</v>
-      </c>
-      <c r="H292" s="3" t="s">
-        <v>1476</v>
-      </c>
-      <c r="I292" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J292" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L292" s="2">
-        <v>19900</v>
-      </c>
-      <c r="M292" s="6">
-        <v>45887</v>
-      </c>
-      <c r="N292" s="2" t="s">
-        <v>1493</v>
-      </c>
+      <c r="A292" s="22"/>
+      <c r="M292" s="6"/>
     </row>
     <row r="293" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A293" s="22">
-        <v>45885</v>
-      </c>
-      <c r="B293" s="7" t="s">
-        <v>1476</v>
-      </c>
-      <c r="C293" s="2" t="s">
-        <v>1494</v>
-      </c>
-      <c r="D293" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E293" s="3" t="s">
-        <v>1495</v>
-      </c>
-      <c r="F293" s="25">
-        <v>150</v>
-      </c>
-      <c r="H293" s="3" t="s">
-        <v>1476</v>
-      </c>
-      <c r="J293" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L293" s="2">
-        <v>2124</v>
-      </c>
-      <c r="N293" s="2" t="s">
-        <v>1493</v>
-      </c>
+      <c r="A293" s="22"/>
     </row>
     <row r="294" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A294" s="22">
-        <v>45886</v>
-      </c>
-      <c r="B294" s="7" t="s">
-        <v>1481</v>
-      </c>
-      <c r="C294" s="2" t="s">
-        <v>1481</v>
-      </c>
-      <c r="D294" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E294" s="3" t="s">
-        <v>774</v>
-      </c>
-      <c r="F294" s="25">
-        <v>300</v>
-      </c>
-      <c r="H294" s="3" t="s">
-        <v>1476</v>
-      </c>
-      <c r="J294" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L294" s="2">
-        <v>10021</v>
-      </c>
-      <c r="N294" s="2" t="s">
-        <v>1493</v>
-      </c>
+      <c r="A294" s="22"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:N283" xr:uid="{0F04922E-3981-41FC-85A3-60DC4C62ADCB}">

</xml_diff>

<commit_message>
Actualización automática: 2025-08-18 13:52:51.005001
</commit_message>
<xml_diff>
--- a/CONTROL REEMBOLSOS.xlsx
+++ b/CONTROL REEMBOLSOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A92566-ADFB-4C79-95D0-473059160968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9AE3AC-CAD1-4599-A9E8-9DE7B793D8C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6179" uniqueCount="1487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6186" uniqueCount="1488">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -4501,6 +4501,9 @@
   </si>
   <si>
     <t>OTROTEST2</t>
+  </si>
+  <si>
+    <t>A la espera de información</t>
   </si>
 </sst>
 </file>
@@ -30106,7 +30109,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A277" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I289" sqref="I289"/>
+      <selection pane="bottomLeft" activeCell="O290" sqref="O290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -41033,7 +41036,36 @@
       </c>
     </row>
     <row r="290" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A290" s="22"/>
+      <c r="A290" s="22">
+        <v>45887</v>
+      </c>
+      <c r="B290" s="7" t="s">
+        <v>1481</v>
+      </c>
+      <c r="C290" s="2" t="s">
+        <v>1481</v>
+      </c>
+      <c r="D290" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E290" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="F290" s="25">
+        <v>150</v>
+      </c>
+      <c r="H290" s="3" t="s">
+        <v>1476</v>
+      </c>
+      <c r="J290" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L290" s="2">
+        <v>201</v>
+      </c>
+      <c r="N290" s="2" t="s">
+        <v>1487</v>
+      </c>
     </row>
     <row r="291" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A291" s="22"/>

</xml_diff>